<commit_message>
다들 SQLD 시험 잘보세요. impl user-api/dummy_data 20251114_jkk(수정중)
</commit_message>
<xml_diff>
--- a/스프링부트 미니프로젝트_prontend_v20251111.xlsx
+++ b/스프링부트 미니프로젝트_prontend_v20251111.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="252">
   <si>
     <t>공통 API</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -218,748 +218,783 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>주문 관리 메서드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문 상세 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문 취소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/products</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/crops</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/crops/{id}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/enable/{id}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/disable/{id}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/products/{id}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REMOVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/orders</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/order/{id}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/order/status/{id}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PATCH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/order/cancel/{id}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/products/search</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ex) /admin/products</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ex) /common/products</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주소 관리 메서드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주소 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주소 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/address/{id}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능</t>
+  </si>
+  <si>
+    <t>페이지 명칭 (URL 예시)</t>
+  </si>
+  <si>
+    <t>역할 및 내용</t>
+  </si>
+  <si>
+    <t>로그인</t>
+  </si>
+  <si>
+    <t>로그인 폼</t>
+  </si>
+  <si>
+    <t>회원가입</t>
+  </si>
+  <si>
+    <t>회원가입 폼</t>
+  </si>
+  <si>
+    <t>index.html</t>
+  </si>
+  <si>
+    <t>메인 페이지, 주요 상품 노출</t>
+  </si>
+  <si>
+    <t>기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>역할 및 내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>common/login.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>common/join.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공통파트 - 회원/로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0. 메인파트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니</t>
+  </si>
+  <si>
+    <t>메인화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니 내역 조회, 수량 변경, 일부/전체 주문 기능</t>
+  </si>
+  <si>
+    <t>상품 목록</t>
+  </si>
+  <si>
+    <t>product/list.html</t>
+  </si>
+  <si>
+    <t>상품 상세</t>
+  </si>
+  <si>
+    <t>product/detail.html</t>
+  </si>
+  <si>
+    <t>모든 농작물 목록, 검색 및 필터 기능 포함</t>
+  </si>
+  <si>
+    <t>단일 농작물 상세 정보, 장바구니 담기, Sold Out 표시</t>
+  </si>
+  <si>
+    <t>주문/결제</t>
+  </si>
+  <si>
+    <t>주문 내역 조회</t>
+  </si>
+  <si>
+    <t>주문 상세</t>
+  </si>
+  <si>
+    <t>특정 주문의 상세 정보</t>
+  </si>
+  <si>
+    <t>배송지 관리</t>
+  </si>
+  <si>
+    <t>배송지 추가/수정/삭제 폼</t>
+  </si>
+  <si>
+    <t>주문 내역 전체 조회, 취소 가능 상태 확인</t>
+  </si>
+  <si>
+    <t>관리자 홈</t>
+  </si>
+  <si>
+    <t>admin/dashboard.html</t>
+  </si>
+  <si>
+    <t>관리자 대시보드 (주요 통계 요약)</t>
+  </si>
+  <si>
+    <t>농작물 등록/관리</t>
+  </si>
+  <si>
+    <t>admin/farm/manage.html</t>
+  </si>
+  <si>
+    <t>농작물 추가/삭제/활성화/비활성화 폼 및 목록</t>
+  </si>
+  <si>
+    <t>상품 등록/관리</t>
+  </si>
+  <si>
+    <t>admin/product/manage.html</t>
+  </si>
+  <si>
+    <t>판매 상품 등록 및 게시 중단 기능 목록</t>
+  </si>
+  <si>
+    <t>주문 조회/처리</t>
+  </si>
+  <si>
+    <t>admin/order/list.html</t>
+  </si>
+  <si>
+    <t>통계/정산</t>
+  </si>
+  <si>
+    <t>admin/stats/main.html</t>
+  </si>
+  <si>
+    <t>일자별/품목별 통계, 정산 내역 조회</t>
+  </si>
+  <si>
+    <t>소비자 주문 목록 조회, 주문 상태 변경, 송장 번호 입력</t>
+  </si>
+  <si>
+    <t>페이지 명칭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 사용자 파트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 관리자 파트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>담당자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결제, 주소지 정보 입력 주문 확정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prontend_admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>branch계정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prontend_common</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prontend_user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* GitHub_NamingRule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강승태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공통화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>base.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공통 헤더/푸터 파트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>허정우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장경국</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>product/cart.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>product/checkout.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>product/orderList.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>product/orderDetail.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>product/address.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자파트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자파트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마이페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품목록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품상세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품제거</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송정보입력(옵션)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결제하기(주문결제)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선택상품주문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체상품주문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송지수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송지추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송지삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문배송관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상세보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문취소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원/로그인</t>
+  </si>
+  <si>
+    <t>회원가입 기능</t>
+  </si>
+  <si>
+    <t>로그인 기능</t>
+  </si>
+  <si>
+    <t>관리자 계정으로 로그인 하면 관리 사이트로 넘어간다.</t>
+  </si>
+  <si>
+    <t>상품/농작물 등록·관리</t>
+  </si>
+  <si>
+    <t>농작물 추가 기능</t>
+  </si>
+  <si>
+    <t>농작물 삭제 기능</t>
+  </si>
+  <si>
+    <t>농작물 재배 활성화/비활성화 기능</t>
+  </si>
+  <si>
+    <t>상품 등록 및 관리</t>
+  </si>
+  <si>
+    <t>창고에 있는 만큼의 농작물을 등록할 수 있다.</t>
+  </si>
+  <si>
+    <t>등록되어 있는 농작물은 게시를 중단할 수 있다.</t>
+  </si>
+  <si>
+    <t>검색/탐색</t>
+  </si>
+  <si>
+    <t>상품 검색 기능 (수확시기 등으로 필터 적용)</t>
+  </si>
+  <si>
+    <t>판매 사이트에 올라와 있는 농작물을 볼 수 있다.</t>
+  </si>
+  <si>
+    <t>장바구니/주문·결제</t>
+  </si>
+  <si>
+    <t>상품 장바구니 기능</t>
+  </si>
+  <si>
+    <t>농작물의 페이지로 들어가 개수를 지정해서 장바구니에 담을 수 있다.</t>
+  </si>
+  <si>
+    <t>장바구니에 있는 농작물의 일부 혹은 전부 구매할 수 있다.</t>
+  </si>
+  <si>
+    <t>주문 조회/처리 - (관리자)</t>
+  </si>
+  <si>
+    <t>소비자가 주문한 농작물 조회 기능</t>
+  </si>
+  <si>
+    <t>주문 상태 변경 기능 → 배송 중으로 변경</t>
+  </si>
+  <si>
+    <t>배송 처리(주문 상품별 송장 번호 및 택배사 정보 입력)</t>
+  </si>
+  <si>
+    <t>주문 조회/처리(취소) - (사용자)</t>
+  </si>
+  <si>
+    <t>재고/노출 관리 - (사용자)</t>
+  </si>
+  <si>
+    <t>통계/정산 - (관리자)</t>
+  </si>
+  <si>
+    <t>농작물 주문 통계 기능 (일자별/품목별 판매시 cnt++)</t>
+  </si>
+  <si>
+    <t>관리자</t>
+  </si>
+  <si>
+    <t>정산(판매 내역, 금액 조회)</t>
+  </si>
+  <si>
+    <t>계정/주소·계좌 관리</t>
+  </si>
+  <si>
+    <t>사용자</t>
+  </si>
+  <si>
+    <t>농가 정보, 계좌 등록</t>
+  </si>
+  <si>
+    <t>물품 상태가 배송 중으로 바뀌기 전에는 주문을 취소할 수 있다.</t>
+  </si>
+  <si>
+    <t>요구 사항 정리</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (품절 표기는 재고/노출과 연관, 배송 맥락과 함께 노출되는 문구로 함께 묶음)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 사용자는 판매 페이지에서 재고가 없는 농작물은 자동으로 sold out 처리된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>●</t>
+  </si>
+  <si>
+    <t>●</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>☞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>항목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기획</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주제선정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>디자인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통합테스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4주차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1주차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>토</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Login/Register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2주차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3주차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요구사항 및 UseCase 설계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB &amp; ERD Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>API 및 각 파트별 기능설계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Display Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSS Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>API Controller</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Service</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manager</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JavaScript/JQuery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MyBatis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User purchase order/cart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shop Item Searching</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Order Managing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crops / Inventories managing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Statistics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Troubleshooting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니에서 아이템 구매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>장바구니에서 아이템 삭제</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문 결과 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/orderlist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 구매 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자는 구매한 물품의 총 개수와 가격을 확인하여 구매할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소비자는 구매한 물품의 총 개수와 가격을 조회할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소비자가 주문한 주문 내역 조회/취소 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/cart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문 목록 조회</t>
+  </si>
+  <si>
+    <t>/orders</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
     <t>장바구니에 아이템 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주문 관리 메서드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주문 상세 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주문 취소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/products</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/crops</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/crops/{id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/enable/{id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/disable/{id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/products/{id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REMOVE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PUT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/orders</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/order/{id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/order/status/{id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PATCH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/order/cancel/{id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/products/search</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ex) /admin/products</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ex) /common/products</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주소 관리 메서드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주소 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/address</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주소 수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/address/{id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기능</t>
-  </si>
-  <si>
-    <t>페이지 명칭 (URL 예시)</t>
-  </si>
-  <si>
-    <t>역할 및 내용</t>
-  </si>
-  <si>
-    <t>로그인</t>
-  </si>
-  <si>
-    <t>로그인 폼</t>
-  </si>
-  <si>
-    <t>회원가입</t>
-  </si>
-  <si>
-    <t>회원가입 폼</t>
-  </si>
-  <si>
-    <t>index.html</t>
-  </si>
-  <si>
-    <t>메인 페이지, 주요 상품 노출</t>
-  </si>
-  <si>
-    <t>기능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>역할 및 내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>common/login.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>common/join.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공통파트 - 회원/로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0. 메인파트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장바구니</t>
-  </si>
-  <si>
-    <t>메인화면</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장바구니 내역 조회, 수량 변경, 일부/전체 주문 기능</t>
-  </si>
-  <si>
-    <t>상품 목록</t>
-  </si>
-  <si>
-    <t>product/list.html</t>
-  </si>
-  <si>
-    <t>상품 상세</t>
-  </si>
-  <si>
-    <t>product/detail.html</t>
-  </si>
-  <si>
-    <t>모든 농작물 목록, 검색 및 필터 기능 포함</t>
-  </si>
-  <si>
-    <t>단일 농작물 상세 정보, 장바구니 담기, Sold Out 표시</t>
-  </si>
-  <si>
-    <t>주문/결제</t>
-  </si>
-  <si>
-    <t>주문 내역 조회</t>
-  </si>
-  <si>
-    <t>주문 상세</t>
-  </si>
-  <si>
-    <t>특정 주문의 상세 정보</t>
-  </si>
-  <si>
-    <t>배송지 관리</t>
-  </si>
-  <si>
-    <t>배송지 추가/수정/삭제 폼</t>
-  </si>
-  <si>
-    <t>주문 내역 전체 조회, 취소 가능 상태 확인</t>
-  </si>
-  <si>
-    <t>관리자 홈</t>
-  </si>
-  <si>
-    <t>admin/dashboard.html</t>
-  </si>
-  <si>
-    <t>관리자 대시보드 (주요 통계 요약)</t>
-  </si>
-  <si>
-    <t>농작물 등록/관리</t>
-  </si>
-  <si>
-    <t>admin/farm/manage.html</t>
-  </si>
-  <si>
-    <t>농작물 추가/삭제/활성화/비활성화 폼 및 목록</t>
-  </si>
-  <si>
-    <t>상품 등록/관리</t>
-  </si>
-  <si>
-    <t>admin/product/manage.html</t>
-  </si>
-  <si>
-    <t>판매 상품 등록 및 게시 중단 기능 목록</t>
-  </si>
-  <si>
-    <t>주문 조회/처리</t>
-  </si>
-  <si>
-    <t>admin/order/list.html</t>
-  </si>
-  <si>
-    <t>통계/정산</t>
-  </si>
-  <si>
-    <t>admin/stats/main.html</t>
-  </si>
-  <si>
-    <t>일자별/품목별 통계, 정산 내역 조회</t>
-  </si>
-  <si>
-    <t>소비자 주문 목록 조회, 주문 상태 변경, 송장 번호 입력</t>
-  </si>
-  <si>
-    <t>페이지 명칭</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 사용자 파트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 관리자 파트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>담당자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결제, 주소지 정보 입력 주문 확정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>prontend_admin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>branch계정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>prontend_common</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>prontend_user</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>* GitHub_NamingRule</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>강승태</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공통화면</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>base.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공통 헤더/푸터 파트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>허정우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장경국</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>product/cart.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>product/checkout.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>product/orderList.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>product/orderDetail.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>product/address.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사용자파트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자파트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마이페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메인페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>대</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>중</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품목록</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품상세</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장바구니</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품제거</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>구매</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>배송정보입력(옵션)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결제하기(주문결제)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>선택상품주문</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전체상품주문</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일반로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원가입</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>배송지수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>배송지추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>배송지삭제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주문배송관리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상세보기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주문취소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주문하기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원/로그인</t>
-  </si>
-  <si>
-    <t>회원가입 기능</t>
-  </si>
-  <si>
-    <t>로그인 기능</t>
-  </si>
-  <si>
-    <t>관리자 계정으로 로그인 하면 관리 사이트로 넘어간다.</t>
-  </si>
-  <si>
-    <t>상품/농작물 등록·관리</t>
-  </si>
-  <si>
-    <t>농작물 추가 기능</t>
-  </si>
-  <si>
-    <t>농작물 삭제 기능</t>
-  </si>
-  <si>
-    <t>농작물 재배 활성화/비활성화 기능</t>
-  </si>
-  <si>
-    <t>상품 등록 및 관리</t>
-  </si>
-  <si>
-    <t>창고에 있는 만큼의 농작물을 등록할 수 있다.</t>
-  </si>
-  <si>
-    <t>등록되어 있는 농작물은 게시를 중단할 수 있다.</t>
-  </si>
-  <si>
-    <t>검색/탐색</t>
-  </si>
-  <si>
-    <t>상품 검색 기능 (수확시기 등으로 필터 적용)</t>
-  </si>
-  <si>
-    <t>판매 사이트에 올라와 있는 농작물을 볼 수 있다.</t>
-  </si>
-  <si>
-    <t>장바구니/주문·결제</t>
-  </si>
-  <si>
-    <t>상품 구매 기능</t>
-  </si>
-  <si>
-    <t>상품 장바구니 기능</t>
-  </si>
-  <si>
-    <t>농작물의 페이지로 들어가 개수를 지정해서 장바구니에 담을 수 있다.</t>
-  </si>
-  <si>
-    <t>장바구니에 있는 농작물의 일부 혹은 전부 구매할 수 있다.</t>
-  </si>
-  <si>
-    <t>주문 조회/처리 - (관리자)</t>
-  </si>
-  <si>
-    <t>소비자가 주문한 농작물 조회 기능</t>
-  </si>
-  <si>
-    <t>주문 상태 변경 기능 → 배송 중으로 변경</t>
-  </si>
-  <si>
-    <t>배송 처리(주문 상품별 송장 번호 및 택배사 정보 입력)</t>
-  </si>
-  <si>
-    <t>주문 조회/처리(취소) - (사용자)</t>
-  </si>
-  <si>
-    <t>소비자가 주문한 주문 내역 조회 기능</t>
-  </si>
-  <si>
-    <t>재고/노출 관리 - (사용자)</t>
-  </si>
-  <si>
-    <t>통계/정산 - (관리자)</t>
-  </si>
-  <si>
-    <t>농작물 주문 통계 기능 (일자별/품목별 판매시 cnt++)</t>
-  </si>
-  <si>
-    <t>관리자</t>
-  </si>
-  <si>
-    <t>정산(판매 내역, 금액 조회)</t>
-  </si>
-  <si>
-    <t>계정/주소·계좌 관리</t>
-  </si>
-  <si>
-    <t>사용자</t>
-  </si>
-  <si>
-    <t>농가 정보, 계좌 등록</t>
-  </si>
-  <si>
-    <t>물품 상태가 배송 중으로 바뀌기 전에는 주문을 취소할 수 있다.</t>
-  </si>
-  <si>
-    <t>요구 사항 정리</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (품절 표기는 재고/노출과 연관, 배송 맥락과 함께 노출되는 문구로 함께 묶음)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일반 사용자는 판매 페이지에서 재고가 없는 농작물은 자동으로 sold out 처리된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>●</t>
-  </si>
-  <si>
-    <t>●</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>☞</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>항목</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>월</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기획</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주제선정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>디자인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기능구현</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>통합테스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4주차</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1주차</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>월</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>목</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>금</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>토</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Login/Register</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2주차</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3주차</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>월</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>목</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>설계</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>요구사항 및 UseCase 설계</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DB &amp; ERD Design</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>API 및 각 파트별 기능설계</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Display Design</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSS Design</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>API Controller</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Service</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Manager</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JavaScript/JQuery</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MyBatis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User purchase order/cart</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shop Item Searching</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Order Managing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Crops / Inventories managing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Statistics</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Troubleshooting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주문 목록 조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1695,37 +1730,37 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2059,7 +2094,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2067,10 +2102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2194,13 +2229,13 @@
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -2208,7 +2243,7 @@
         <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -2219,7 +2254,7 @@
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
@@ -2301,7 +2336,7 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -2315,7 +2350,7 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -2326,7 +2361,7 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -2337,7 +2372,7 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
@@ -2355,13 +2390,13 @@
         <v>14</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -2369,10 +2404,10 @@
         <v>15</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -2380,10 +2415,10 @@
         <v>16</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2398,7 +2433,7 @@
         <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>20</v>
@@ -2406,10 +2441,10 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
         <v>20</v>
@@ -2420,10 +2455,10 @@
         <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
@@ -2513,7 +2548,7 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>251</v>
       </c>
       <c r="B43" t="s">
         <v>37</v>
@@ -2524,7 +2559,7 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>239</v>
       </c>
       <c r="B44" t="s">
         <v>36</v>
@@ -2533,19 +2568,30 @@
         <v>8</v>
       </c>
     </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>238</v>
+      </c>
+      <c r="B45" t="s">
+        <v>247</v>
+      </c>
+      <c r="C45" t="s">
+        <v>240</v>
+      </c>
+    </row>
     <row r="47" spans="1:15" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="3"/>
     </row>
     <row r="48" spans="1:15" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>241</v>
+      </c>
+      <c r="B48" t="s">
         <v>242</v>
-      </c>
-      <c r="B48" t="s">
-        <v>51</v>
       </c>
       <c r="C48" t="s">
         <v>20</v>
@@ -2553,52 +2599,63 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>248</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>249</v>
       </c>
       <c r="C49" t="s">
-        <v>20</v>
+        <v>250</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B50" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C50" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" t="s">
         <v>59</v>
       </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="3"/>
-    </row>
-    <row r="53" spans="1:3" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="C54" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>60</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B55" t="s">
         <v>61</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>62</v>
-      </c>
-      <c r="B54" t="s">
-        <v>63</v>
-      </c>
-      <c r="C54" s="4" t="s">
+      <c r="C55" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2637,7 +2694,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="65" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
@@ -2690,91 +2747,91 @@
     </row>
     <row r="5" spans="1:19" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>75</v>
-      </c>
       <c r="D6" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D7" s="70" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>122</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>124</v>
       </c>
       <c r="D8" s="70"/>
       <c r="G8" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D9" s="70"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D10" s="70"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="65" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B12" s="65"/>
       <c r="C12" s="65"/>
@@ -2827,163 +2884,163 @@
     </row>
     <row r="15" spans="1:19" ht="24" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>66</v>
-      </c>
       <c r="D16" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="Q16" s="69" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="R16" s="69"/>
       <c r="S16" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D17" s="70" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="D18" s="70"/>
       <c r="S18" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="D19" s="70"/>
       <c r="Q19" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="S19" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D20" s="70"/>
       <c r="S20" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D21" s="70"/>
       <c r="S21" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D22" s="70"/>
       <c r="S22" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D23" s="70"/>
       <c r="Q23" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="S23" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="S24" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="65" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B25" s="65"/>
       <c r="C25" s="65"/>
@@ -3000,10 +3057,10 @@
       <c r="N25" s="65"/>
       <c r="O25" s="65"/>
       <c r="Q25" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="S25" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
@@ -3023,7 +3080,7 @@
       <c r="N26" s="65"/>
       <c r="O26" s="65"/>
       <c r="S26" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
@@ -3043,111 +3100,111 @@
       <c r="N27" s="65"/>
       <c r="O27" s="65"/>
       <c r="Q27" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="S27" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="24" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="Q28" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="S28" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>66</v>
-      </c>
       <c r="D29" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="S29" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>98</v>
-      </c>
       <c r="D30" s="70" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="S30" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="D31" s="70"/>
       <c r="R31" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="S31" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="D32" s="70"/>
       <c r="S32" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D33" s="70"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="D34" s="70"/>
     </row>
@@ -3169,9 +3226,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:X28"/>
+  <dimension ref="B3:X29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3180,7 +3239,7 @@
   <sheetData>
     <row r="3" spans="2:24" ht="72" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="71" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C3" s="71"/>
       <c r="D3" s="71"/>
@@ -3229,10 +3288,10 @@
     </row>
     <row r="5" spans="2:24" ht="24" x14ac:dyDescent="0.3">
       <c r="D5" s="25" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
@@ -3243,10 +3302,10 @@
       <c r="L5" s="20"/>
       <c r="M5" s="20"/>
       <c r="N5" s="26" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="O5" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="P5" s="20"/>
       <c r="Q5" s="20"/>
@@ -3260,10 +3319,10 @@
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
       <c r="D6" s="18"/>
       <c r="E6" s="26" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
@@ -3274,10 +3333,10 @@
       <c r="M6" s="20"/>
       <c r="N6" s="20"/>
       <c r="O6" s="26" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="P6" s="27" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="Q6" s="20"/>
       <c r="R6" s="20"/>
@@ -3290,10 +3349,10 @@
     <row r="7" spans="2:24" x14ac:dyDescent="0.3">
       <c r="D7" s="18"/>
       <c r="E7" s="26" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
@@ -3305,7 +3364,7 @@
       <c r="N7" s="20"/>
       <c r="O7" s="20"/>
       <c r="P7" s="20" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="Q7" s="20"/>
       <c r="R7" s="20"/>
@@ -3319,7 +3378,7 @@
       <c r="D8" s="18"/>
       <c r="E8" s="26"/>
       <c r="F8" s="20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
@@ -3331,7 +3390,7 @@
       <c r="N8" s="20"/>
       <c r="O8" s="20"/>
       <c r="P8" s="20" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="Q8" s="20"/>
       <c r="R8" s="20"/>
@@ -3365,10 +3424,10 @@
     </row>
     <row r="10" spans="2:24" ht="24" x14ac:dyDescent="0.3">
       <c r="D10" s="25" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
@@ -3379,10 +3438,10 @@
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="26" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="P10" s="20"/>
       <c r="Q10" s="20"/>
@@ -3396,10 +3455,10 @@
     <row r="11" spans="2:24" x14ac:dyDescent="0.3">
       <c r="D11" s="18"/>
       <c r="E11" s="26" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
@@ -3410,10 +3469,10 @@
       <c r="M11" s="20"/>
       <c r="N11" s="20"/>
       <c r="O11" s="26" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="P11" s="27" t="s">
-        <v>185</v>
+        <v>246</v>
       </c>
       <c r="Q11" s="20"/>
       <c r="R11" s="20"/>
@@ -3426,10 +3485,10 @@
     <row r="12" spans="2:24" x14ac:dyDescent="0.3">
       <c r="D12" s="18"/>
       <c r="E12" s="26" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
@@ -3440,8 +3499,8 @@
       <c r="M12" s="20"/>
       <c r="N12" s="20"/>
       <c r="O12" s="20"/>
-      <c r="P12" s="20" t="s">
-        <v>194</v>
+      <c r="P12" s="14" t="s">
+        <v>245</v>
       </c>
       <c r="Q12" s="20"/>
       <c r="R12" s="20"/>
@@ -3454,10 +3513,10 @@
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="D13" s="18"/>
       <c r="E13" s="26" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
@@ -3467,8 +3526,10 @@
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
       <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="20" t="s">
+        <v>190</v>
+      </c>
       <c r="Q13" s="20"/>
       <c r="R13" s="20"/>
       <c r="S13" s="20"/>
@@ -3477,13 +3538,13 @@
       <c r="V13" s="20"/>
       <c r="W13" s="21"/>
     </row>
-    <row r="14" spans="2:24" ht="24" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
       <c r="D14" s="18"/>
       <c r="E14" s="26" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
@@ -3492,13 +3553,6 @@
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
-      <c r="N14" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="O14" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="P14" s="20"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="20"/>
       <c r="S14" s="20"/>
@@ -3507,11 +3561,11 @@
       <c r="V14" s="20"/>
       <c r="W14" s="21"/>
     </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:24" ht="24" x14ac:dyDescent="0.3">
       <c r="D15" s="18"/>
       <c r="E15" s="20"/>
       <c r="F15" s="20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
@@ -3520,13 +3574,13 @@
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="P15" s="27" t="s">
-        <v>197</v>
-      </c>
+      <c r="N15" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="O15" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="P15" s="20"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="20"/>
       <c r="S15" s="20"/>
@@ -3539,7 +3593,7 @@
       <c r="D16" s="18"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
@@ -3549,9 +3603,11 @@
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
       <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20" t="s">
+      <c r="O16" s="26" t="s">
         <v>196</v>
+      </c>
+      <c r="P16" s="27" t="s">
+        <v>193</v>
       </c>
       <c r="Q16" s="20"/>
       <c r="R16" s="20"/>
@@ -3574,7 +3630,9 @@
       <c r="M17" s="20"/>
       <c r="N17" s="20"/>
       <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
+      <c r="P17" s="20" t="s">
+        <v>192</v>
+      </c>
       <c r="Q17" s="20"/>
       <c r="R17" s="20"/>
       <c r="S17" s="20"/>
@@ -3585,10 +3643,10 @@
     </row>
     <row r="18" spans="4:23" ht="24" x14ac:dyDescent="0.3">
       <c r="D18" s="25" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
@@ -3598,12 +3656,8 @@
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
       <c r="M18" s="20"/>
-      <c r="N18" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="O18" s="19" t="s">
-        <v>187</v>
-      </c>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
       <c r="P18" s="20"/>
       <c r="Q18" s="20"/>
       <c r="R18" s="20"/>
@@ -3613,13 +3667,13 @@
       <c r="V18" s="20"/>
       <c r="W18" s="21"/>
     </row>
-    <row r="19" spans="4:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:23" ht="24" x14ac:dyDescent="0.3">
       <c r="D19" s="18"/>
       <c r="E19" s="26" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
@@ -3628,13 +3682,13 @@
       <c r="K19" s="20"/>
       <c r="L19" s="20"/>
       <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="P19" s="27" t="s">
-        <v>188</v>
-      </c>
+      <c r="N19" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="O19" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="P19" s="20"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="20"/>
       <c r="S19" s="20"/>
@@ -3647,7 +3701,7 @@
       <c r="D20" s="18"/>
       <c r="E20" s="20"/>
       <c r="F20" s="27" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
@@ -3657,9 +3711,11 @@
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
       <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20" t="s">
-        <v>189</v>
+      <c r="O20" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="P20" s="27" t="s">
+        <v>184</v>
       </c>
       <c r="Q20" s="20"/>
       <c r="R20" s="20"/>
@@ -3681,11 +3737,9 @@
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
       <c r="N21" s="20"/>
-      <c r="O21" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="P21" s="27" t="s">
-        <v>190</v>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20" t="s">
+        <v>185</v>
       </c>
       <c r="Q21" s="20"/>
       <c r="R21" s="20"/>
@@ -3697,10 +3751,10 @@
     </row>
     <row r="22" spans="4:23" ht="24" x14ac:dyDescent="0.3">
       <c r="D22" s="25" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
@@ -3711,8 +3765,12 @@
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
       <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
+      <c r="O22" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="P22" s="27" t="s">
+        <v>186</v>
+      </c>
       <c r="Q22" s="20"/>
       <c r="R22" s="20"/>
       <c r="S22" s="20"/>
@@ -3721,13 +3779,13 @@
       <c r="V22" s="20"/>
       <c r="W22" s="21"/>
     </row>
-    <row r="23" spans="4:23" ht="24" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D23" s="18"/>
       <c r="E23" s="26" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
@@ -3736,12 +3794,8 @@
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
       <c r="M23" s="20"/>
-      <c r="N23" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="O23" s="19" t="s">
-        <v>191</v>
-      </c>
+      <c r="N23" s="20"/>
+      <c r="O23" s="20"/>
       <c r="P23" s="20"/>
       <c r="Q23" s="20"/>
       <c r="R23" s="20"/>
@@ -3751,13 +3805,11 @@
       <c r="V23" s="20"/>
       <c r="W23" s="21"/>
     </row>
-    <row r="24" spans="4:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:23" ht="24" x14ac:dyDescent="0.3">
       <c r="D24" s="18"/>
-      <c r="E24" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="F24" s="27" t="s">
-        <v>177</v>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20" t="s">
+        <v>175</v>
       </c>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
@@ -3766,11 +3818,13 @@
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="20"/>
-      <c r="P24" s="20" t="s">
-        <v>192</v>
-      </c>
+      <c r="N24" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="O24" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="P24" s="20"/>
       <c r="Q24" s="20"/>
       <c r="R24" s="20"/>
       <c r="S24" s="20"/>
@@ -3783,7 +3837,7 @@
       <c r="D25" s="18"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
@@ -3793,11 +3847,9 @@
       <c r="L25" s="20"/>
       <c r="M25" s="20"/>
       <c r="N25" s="20"/>
-      <c r="O25" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="P25" s="27" t="s">
-        <v>93</v>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20" t="s">
+        <v>188</v>
       </c>
       <c r="Q25" s="20"/>
       <c r="R25" s="20"/>
@@ -3809,9 +3861,11 @@
     </row>
     <row r="26" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D26" s="18"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20" t="s">
-        <v>179</v>
+      <c r="E26" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>243</v>
       </c>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
@@ -3821,9 +3875,11 @@
       <c r="L26" s="20"/>
       <c r="M26" s="20"/>
       <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20" t="s">
-        <v>189</v>
+      <c r="O26" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="P26" s="27" t="s">
+        <v>91</v>
       </c>
       <c r="Q26" s="20"/>
       <c r="R26" s="20"/>
@@ -3835,8 +3891,9 @@
     </row>
     <row r="27" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D27" s="18"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
+      <c r="F27" s="14" t="s">
+        <v>244</v>
+      </c>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
@@ -3845,11 +3902,9 @@
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
       <c r="N27" s="20"/>
-      <c r="O27" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="P27" s="27" t="s">
-        <v>193</v>
+      <c r="O27" s="20"/>
+      <c r="P27" s="20" t="s">
+        <v>185</v>
       </c>
       <c r="Q27" s="20"/>
       <c r="R27" s="20"/>
@@ -3859,27 +3914,51 @@
       <c r="V27" s="20"/>
       <c r="W27" s="21"/>
     </row>
-    <row r="28" spans="4:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D28" s="22"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="23"/>
-      <c r="T28" s="23"/>
-      <c r="U28" s="23"/>
-      <c r="V28" s="23"/>
-      <c r="W28" s="24"/>
+    <row r="28" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D28" s="18"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="P28" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q28" s="20"/>
+      <c r="R28" s="20"/>
+      <c r="S28" s="20"/>
+      <c r="T28" s="20"/>
+      <c r="U28" s="20"/>
+      <c r="V28" s="20"/>
+      <c r="W28" s="21"/>
+    </row>
+    <row r="29" spans="4:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D29" s="22"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="23"/>
+      <c r="U29" s="23"/>
+      <c r="V29" s="23"/>
+      <c r="W29" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3899,7 +3978,7 @@
       <pane xSplit="30" ySplit="23" topLeftCell="AE24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AE1" sqref="AE1"/>
       <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3915,143 +3994,143 @@
     <row r="1" spans="2:31" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:31" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="79" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" s="72" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="72" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="75" t="s">
+        <v>215</v>
+      </c>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="72" t="s">
+        <v>216</v>
+      </c>
+      <c r="S3" s="73"/>
+      <c r="T3" s="73"/>
+      <c r="U3" s="73"/>
+      <c r="V3" s="73"/>
+      <c r="W3" s="73"/>
+      <c r="X3" s="74"/>
+      <c r="Y3" s="76" t="s">
+        <v>205</v>
+      </c>
+      <c r="Z3" s="77"/>
+      <c r="AA3" s="77"/>
+      <c r="AB3" s="77"/>
+      <c r="AC3" s="77"/>
+      <c r="AD3" s="77"/>
+      <c r="AE3" s="78"/>
+    </row>
+    <row r="4" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="80"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="63" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4" s="63" t="s">
+        <v>208</v>
+      </c>
+      <c r="F4" s="63" t="s">
+        <v>209</v>
+      </c>
+      <c r="G4" s="63" t="s">
+        <v>210</v>
+      </c>
+      <c r="H4" s="63" t="s">
+        <v>211</v>
+      </c>
+      <c r="I4" s="63" t="s">
+        <v>212</v>
+      </c>
+      <c r="J4" s="63" t="s">
+        <v>217</v>
+      </c>
+      <c r="K4" s="63" t="s">
+        <v>218</v>
+      </c>
+      <c r="L4" s="63" t="s">
+        <v>219</v>
+      </c>
+      <c r="M4" s="63" t="s">
+        <v>209</v>
+      </c>
+      <c r="N4" s="63" t="s">
+        <v>220</v>
+      </c>
+      <c r="O4" s="63" t="s">
+        <v>211</v>
+      </c>
+      <c r="P4" s="63" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q4" s="63" t="s">
+        <v>217</v>
+      </c>
+      <c r="R4" s="63" t="s">
+        <v>199</v>
+      </c>
+      <c r="S4" s="63" t="s">
+        <v>208</v>
+      </c>
+      <c r="T4" s="63" t="s">
+        <v>209</v>
+      </c>
+      <c r="U4" s="63" t="s">
+        <v>210</v>
+      </c>
+      <c r="V4" s="63" t="s">
+        <v>211</v>
+      </c>
+      <c r="W4" s="63" t="s">
+        <v>212</v>
+      </c>
+      <c r="X4" s="63" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y4" s="63" t="s">
+        <v>218</v>
+      </c>
+      <c r="Z4" s="63" t="s">
+        <v>208</v>
+      </c>
+      <c r="AA4" s="63" t="s">
+        <v>209</v>
+      </c>
+      <c r="AB4" s="63" t="s">
+        <v>210</v>
+      </c>
+      <c r="AC4" s="63" t="s">
+        <v>211</v>
+      </c>
+      <c r="AD4" s="63" t="s">
+        <v>212</v>
+      </c>
+      <c r="AE4" s="63" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="79" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" s="64" t="s">
         <v>201</v>
-      </c>
-      <c r="C3" s="75" t="s">
-        <v>202</v>
-      </c>
-      <c r="D3" s="75" t="s">
-        <v>210</v>
-      </c>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="78" t="s">
-        <v>219</v>
-      </c>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="76"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="75" t="s">
-        <v>220</v>
-      </c>
-      <c r="S3" s="76"/>
-      <c r="T3" s="76"/>
-      <c r="U3" s="76"/>
-      <c r="V3" s="76"/>
-      <c r="W3" s="76"/>
-      <c r="X3" s="77"/>
-      <c r="Y3" s="79" t="s">
-        <v>209</v>
-      </c>
-      <c r="Z3" s="80"/>
-      <c r="AA3" s="80"/>
-      <c r="AB3" s="80"/>
-      <c r="AC3" s="80"/>
-      <c r="AD3" s="80"/>
-      <c r="AE3" s="81"/>
-    </row>
-    <row r="4" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="73"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="63" t="s">
-        <v>211</v>
-      </c>
-      <c r="E4" s="63" t="s">
-        <v>212</v>
-      </c>
-      <c r="F4" s="63" t="s">
-        <v>213</v>
-      </c>
-      <c r="G4" s="63" t="s">
-        <v>214</v>
-      </c>
-      <c r="H4" s="63" t="s">
-        <v>215</v>
-      </c>
-      <c r="I4" s="63" t="s">
-        <v>216</v>
-      </c>
-      <c r="J4" s="63" t="s">
-        <v>221</v>
-      </c>
-      <c r="K4" s="63" t="s">
-        <v>222</v>
-      </c>
-      <c r="L4" s="63" t="s">
-        <v>223</v>
-      </c>
-      <c r="M4" s="63" t="s">
-        <v>213</v>
-      </c>
-      <c r="N4" s="63" t="s">
-        <v>224</v>
-      </c>
-      <c r="O4" s="63" t="s">
-        <v>215</v>
-      </c>
-      <c r="P4" s="63" t="s">
-        <v>216</v>
-      </c>
-      <c r="Q4" s="63" t="s">
-        <v>221</v>
-      </c>
-      <c r="R4" s="63" t="s">
-        <v>203</v>
-      </c>
-      <c r="S4" s="63" t="s">
-        <v>212</v>
-      </c>
-      <c r="T4" s="63" t="s">
-        <v>213</v>
-      </c>
-      <c r="U4" s="63" t="s">
-        <v>214</v>
-      </c>
-      <c r="V4" s="63" t="s">
-        <v>215</v>
-      </c>
-      <c r="W4" s="63" t="s">
-        <v>216</v>
-      </c>
-      <c r="X4" s="63" t="s">
-        <v>217</v>
-      </c>
-      <c r="Y4" s="63" t="s">
-        <v>222</v>
-      </c>
-      <c r="Z4" s="63" t="s">
-        <v>212</v>
-      </c>
-      <c r="AA4" s="63" t="s">
-        <v>213</v>
-      </c>
-      <c r="AB4" s="63" t="s">
-        <v>214</v>
-      </c>
-      <c r="AC4" s="63" t="s">
-        <v>215</v>
-      </c>
-      <c r="AD4" s="63" t="s">
-        <v>216</v>
-      </c>
-      <c r="AE4" s="63" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="5" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="72" t="s">
-        <v>204</v>
-      </c>
-      <c r="C5" s="64" t="s">
-        <v>205</v>
       </c>
       <c r="D5" s="42"/>
       <c r="E5" s="43"/>
@@ -4083,9 +4162,9 @@
       <c r="AE5" s="45"/>
     </row>
     <row r="6" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="73"/>
+      <c r="B6" s="80"/>
       <c r="C6" s="64" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="33"/>
@@ -4117,11 +4196,11 @@
       <c r="AE6" s="34"/>
     </row>
     <row r="7" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="72" t="s">
-        <v>225</v>
+      <c r="B7" s="79" t="s">
+        <v>221</v>
       </c>
       <c r="C7" s="64" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D7" s="42"/>
       <c r="E7" s="43"/>
@@ -4153,9 +4232,9 @@
       <c r="AE7" s="45"/>
     </row>
     <row r="8" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="73"/>
+      <c r="B8" s="80"/>
       <c r="C8" s="64" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="33"/>
@@ -4187,11 +4266,11 @@
       <c r="AE8" s="34"/>
     </row>
     <row r="9" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="72" t="s">
-        <v>206</v>
+      <c r="B9" s="79" t="s">
+        <v>202</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D9" s="42"/>
       <c r="E9" s="43"/>
@@ -4223,9 +4302,9 @@
       <c r="AE9" s="45"/>
     </row>
     <row r="10" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="73"/>
+      <c r="B10" s="80"/>
       <c r="C10" s="64" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="33"/>
@@ -4257,11 +4336,11 @@
       <c r="AE10" s="34"/>
     </row>
     <row r="11" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="72" t="s">
-        <v>207</v>
+      <c r="B11" s="79" t="s">
+        <v>203</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D11" s="42"/>
       <c r="E11" s="43"/>
@@ -4293,9 +4372,9 @@
       <c r="AE11" s="45"/>
     </row>
     <row r="12" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="74"/>
+      <c r="B12" s="82"/>
       <c r="C12" s="64" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D12" s="30"/>
       <c r="E12" s="28"/>
@@ -4327,9 +4406,9 @@
       <c r="AE12" s="31"/>
     </row>
     <row r="13" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="74"/>
+      <c r="B13" s="82"/>
       <c r="C13" s="64" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D13" s="30"/>
       <c r="E13" s="28"/>
@@ -4361,9 +4440,9 @@
       <c r="AE13" s="31"/>
     </row>
     <row r="14" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="74"/>
+      <c r="B14" s="82"/>
       <c r="C14" s="64" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D14" s="30"/>
       <c r="E14" s="28"/>
@@ -4395,9 +4474,9 @@
       <c r="AE14" s="31"/>
     </row>
     <row r="15" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="73"/>
+      <c r="B15" s="80"/>
       <c r="C15" s="64" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D15" s="32"/>
       <c r="E15" s="33"/>
@@ -4429,11 +4508,11 @@
       <c r="AE15" s="34"/>
     </row>
     <row r="16" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="72" t="s">
-        <v>208</v>
+      <c r="B16" s="79" t="s">
+        <v>204</v>
       </c>
       <c r="C16" s="64" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D16" s="42"/>
       <c r="E16" s="43"/>
@@ -4465,9 +4544,9 @@
       <c r="AE16" s="45"/>
     </row>
     <row r="17" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="74"/>
+      <c r="B17" s="82"/>
       <c r="C17" s="64" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D17" s="30"/>
       <c r="E17" s="28"/>
@@ -4499,9 +4578,9 @@
       <c r="AE17" s="31"/>
     </row>
     <row r="18" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="74"/>
+      <c r="B18" s="82"/>
       <c r="C18" s="64" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D18" s="30"/>
       <c r="E18" s="28"/>
@@ -4533,9 +4612,9 @@
       <c r="AE18" s="31"/>
     </row>
     <row r="19" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="74"/>
+      <c r="B19" s="82"/>
       <c r="C19" s="64" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D19" s="30"/>
       <c r="E19" s="28"/>
@@ -4567,9 +4646,9 @@
       <c r="AE19" s="31"/>
     </row>
     <row r="20" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="74"/>
+      <c r="B20" s="82"/>
       <c r="C20" s="64" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D20" s="30"/>
       <c r="E20" s="28"/>
@@ -4601,9 +4680,9 @@
       <c r="AE20" s="31"/>
     </row>
     <row r="21" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="74"/>
+      <c r="B21" s="82"/>
       <c r="C21" s="64" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D21" s="30"/>
       <c r="E21" s="28"/>
@@ -4635,9 +4714,9 @@
       <c r="AE21" s="31"/>
     </row>
     <row r="22" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="73"/>
+      <c r="B22" s="80"/>
       <c r="C22" s="64" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D22" s="32"/>
       <c r="E22" s="33"/>
@@ -4671,17 +4750,17 @@
     <row r="23" spans="2:31" ht="11.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="B16:B22"/>
     <mergeCell ref="D3:J3"/>
     <mergeCell ref="K3:Q3"/>
     <mergeCell ref="R3:X3"/>
     <mergeCell ref="Y3:AE3"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="B16:B22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
impl user-order connection & testing 20251117_jkk
</commit_message>
<xml_diff>
--- a/스프링부트 미니프로젝트_prontend_v20251111.xlsx
+++ b/스프링부트 미니프로젝트_prontend_v20251111.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name=" API" sheetId="1" r:id="rId1"/>
-    <sheet name="ProntEnd" sheetId="2" r:id="rId2"/>
-    <sheet name="요구사항 정리" sheetId="3" r:id="rId3"/>
-    <sheet name="일정관리" sheetId="4" r:id="rId4"/>
+    <sheet name="팀프로젝트" sheetId="6" r:id="rId1"/>
+    <sheet name=" API" sheetId="1" r:id="rId2"/>
+    <sheet name="ProntEnd" sheetId="2" r:id="rId3"/>
+    <sheet name="요구사항 정리" sheetId="3" r:id="rId4"/>
+    <sheet name="일정관리" sheetId="4" r:id="rId5"/>
+    <sheet name="이력관리" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">일정관리!$A$1:$AF$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">일정관리!$A$1:$AF$23</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,28 +39,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="310">
   <si>
     <t>공통 API</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그아웃</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/login</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/logout</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>행동</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -74,35 +61,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>농작물 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>농작물 삭제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>농작물 활성화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>농작물 비활성화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>농작물 관리 메서드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품 등록</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품 수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품 삭제</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -178,14 +137,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ex) /admin/addCrop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>계정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/account</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -194,10 +145,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ex) /account/login</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>장바구니 관리 메서드</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -234,768 +181,1005 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/crops</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/crops/{id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/enable/{id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/disable/{id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/products/{id}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>REMOVE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>/orders</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/order/{id}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/order/status/{id}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PATCH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/order/cancel/{id}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/products/search</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ex) /common/products</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주소 관리 메서드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주소 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주소 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/address/{id}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능</t>
+  </si>
+  <si>
+    <t>페이지 명칭 (URL 예시)</t>
+  </si>
+  <si>
+    <t>역할 및 내용</t>
+  </si>
+  <si>
+    <t>로그인</t>
+  </si>
+  <si>
+    <t>로그인 폼</t>
+  </si>
+  <si>
+    <t>회원가입</t>
+  </si>
+  <si>
+    <t>회원가입 폼</t>
+  </si>
+  <si>
+    <t>index.html</t>
+  </si>
+  <si>
+    <t>메인 페이지, 주요 상품 노출</t>
+  </si>
+  <si>
+    <t>기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>역할 및 내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>common/login.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>common/join.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공통파트 - 회원/로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0. 메인파트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니</t>
+  </si>
+  <si>
+    <t>메인화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니 내역 조회, 수량 변경, 일부/전체 주문 기능</t>
+  </si>
+  <si>
+    <t>상품 목록</t>
+  </si>
+  <si>
+    <t>product/list.html</t>
+  </si>
+  <si>
+    <t>상품 상세</t>
+  </si>
+  <si>
+    <t>product/detail.html</t>
+  </si>
+  <si>
+    <t>모든 농작물 목록, 검색 및 필터 기능 포함</t>
+  </si>
+  <si>
+    <t>단일 농작물 상세 정보, 장바구니 담기, Sold Out 표시</t>
+  </si>
+  <si>
+    <t>주문/결제</t>
+  </si>
+  <si>
+    <t>주문 내역 조회</t>
+  </si>
+  <si>
+    <t>주문 상세</t>
+  </si>
+  <si>
+    <t>특정 주문의 상세 정보</t>
+  </si>
+  <si>
+    <t>배송지 관리</t>
+  </si>
+  <si>
+    <t>배송지 추가/수정/삭제 폼</t>
+  </si>
+  <si>
+    <t>주문 내역 전체 조회, 취소 가능 상태 확인</t>
+  </si>
+  <si>
+    <t>관리자 홈</t>
+  </si>
+  <si>
+    <t>admin/dashboard.html</t>
+  </si>
+  <si>
+    <t>관리자 대시보드 (주요 통계 요약)</t>
+  </si>
+  <si>
+    <t>농작물 등록/관리</t>
+  </si>
+  <si>
+    <t>admin/farm/manage.html</t>
+  </si>
+  <si>
+    <t>농작물 추가/삭제/활성화/비활성화 폼 및 목록</t>
+  </si>
+  <si>
+    <t>상품 등록/관리</t>
+  </si>
+  <si>
+    <t>admin/product/manage.html</t>
+  </si>
+  <si>
+    <t>판매 상품 등록 및 게시 중단 기능 목록</t>
+  </si>
+  <si>
+    <t>주문 조회/처리</t>
+  </si>
+  <si>
+    <t>admin/order/list.html</t>
+  </si>
+  <si>
+    <t>통계/정산</t>
+  </si>
+  <si>
+    <t>admin/stats/main.html</t>
+  </si>
+  <si>
+    <t>일자별/품목별 통계, 정산 내역 조회</t>
+  </si>
+  <si>
+    <t>소비자 주문 목록 조회, 주문 상태 변경, 송장 번호 입력</t>
+  </si>
+  <si>
+    <t>페이지 명칭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 사용자 파트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 관리자 파트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>담당자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결제, 주소지 정보 입력 주문 확정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prontend_admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>branch계정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prontend_common</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prontend_user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* GitHub_NamingRule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강승태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공통화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>base.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공통 헤더/푸터 파트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>허정우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장경국</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>product/cart.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>product/checkout.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>product/orderList.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>product/orderDetail.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>product/address.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자파트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자파트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마이페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품목록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품상세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품제거</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송정보입력(옵션)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결제하기(주문결제)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선택상품주문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체상품주문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송지수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송지추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송지삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문배송관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상세보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문취소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원/로그인</t>
+  </si>
+  <si>
+    <t>회원가입 기능</t>
+  </si>
+  <si>
+    <t>로그인 기능</t>
+  </si>
+  <si>
+    <t>관리자 계정으로 로그인 하면 관리 사이트로 넘어간다.</t>
+  </si>
+  <si>
+    <t>상품/농작물 등록·관리</t>
+  </si>
+  <si>
+    <t>농작물 추가 기능</t>
+  </si>
+  <si>
+    <t>농작물 삭제 기능</t>
+  </si>
+  <si>
+    <t>농작물 재배 활성화/비활성화 기능</t>
+  </si>
+  <si>
+    <t>상품 등록 및 관리</t>
+  </si>
+  <si>
+    <t>창고에 있는 만큼의 농작물을 등록할 수 있다.</t>
+  </si>
+  <si>
+    <t>등록되어 있는 농작물은 게시를 중단할 수 있다.</t>
+  </si>
+  <si>
+    <t>검색/탐색</t>
+  </si>
+  <si>
+    <t>상품 검색 기능 (수확시기 등으로 필터 적용)</t>
+  </si>
+  <si>
+    <t>판매 사이트에 올라와 있는 농작물을 볼 수 있다.</t>
+  </si>
+  <si>
+    <t>장바구니/주문·결제</t>
+  </si>
+  <si>
+    <t>상품 장바구니 기능</t>
+  </si>
+  <si>
+    <t>농작물의 페이지로 들어가 개수를 지정해서 장바구니에 담을 수 있다.</t>
+  </si>
+  <si>
+    <t>장바구니에 있는 농작물의 일부 혹은 전부 구매할 수 있다.</t>
+  </si>
+  <si>
+    <t>주문 조회/처리 - (관리자)</t>
+  </si>
+  <si>
+    <t>소비자가 주문한 농작물 조회 기능</t>
+  </si>
+  <si>
+    <t>주문 상태 변경 기능 → 배송 중으로 변경</t>
+  </si>
+  <si>
+    <t>배송 처리(주문 상품별 송장 번호 및 택배사 정보 입력)</t>
+  </si>
+  <si>
+    <t>주문 조회/처리(취소) - (사용자)</t>
+  </si>
+  <si>
+    <t>재고/노출 관리 - (사용자)</t>
+  </si>
+  <si>
+    <t>통계/정산 - (관리자)</t>
+  </si>
+  <si>
+    <t>농작물 주문 통계 기능 (일자별/품목별 판매시 cnt++)</t>
+  </si>
+  <si>
+    <t>관리자</t>
+  </si>
+  <si>
+    <t>정산(판매 내역, 금액 조회)</t>
+  </si>
+  <si>
+    <t>계정/주소·계좌 관리</t>
+  </si>
+  <si>
+    <t>사용자</t>
+  </si>
+  <si>
+    <t>농가 정보, 계좌 등록</t>
+  </si>
+  <si>
+    <t>물품 상태가 배송 중으로 바뀌기 전에는 주문을 취소할 수 있다.</t>
+  </si>
+  <si>
+    <t>요구 사항 정리</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (품절 표기는 재고/노출과 연관, 배송 맥락과 함께 노출되는 문구로 함께 묶음)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 사용자는 판매 페이지에서 재고가 없는 농작물은 자동으로 sold out 처리된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>●</t>
+  </si>
+  <si>
+    <t>●</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>☞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>항목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기획</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주제선정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>디자인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통합테스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4주차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1주차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>토</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Login/Register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2주차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3주차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요구사항 및 UseCase 설계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB &amp; ERD Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>API 및 각 파트별 기능설계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Display Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSS Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>API Controller</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Service</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manager</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JavaScript/JQuery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MyBatis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User purchase order/cart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shop Item Searching</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Order Managing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crops / Inventories managing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Statistics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Troubleshooting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니에서 아이템 구매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니에서 아이템 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문 결과 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/orderlist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 구매 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자는 구매한 물품의 총 개수와 가격을 확인하여 구매할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소비자는 구매한 물품의 총 개수와 가격을 조회할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소비자가 주문한 주문 내역 조회/취소 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/cart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문 목록 조회</t>
+  </si>
+  <si>
+    <t>/orders</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>장바구니에 아이템 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 주소 관리 메서드에 주소 삭제 메서드 추가</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 어드민 관리 페이지 입장 url 및 controller 방식을 REST API 방식으로 수정한 api 추가</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 소비자 주소 관리 메서드 Controller와 RestController 방식으로 분리</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 어드민 농작물 관리 페이지 및 controller 방식을 REST API 방식으로 수정</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 어드민 농장 주소 관리 API 구현</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 작물 및 창고 항목 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 회원가입 ID 중복 확인 및 처리 기능 구현 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 상품관리 페이지 등 유효성 검사 기능 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 로그인 관리 기능 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 주소 관리 기능 구현 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 소비자 주문 관리 API 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 소비자 구매/장바구니 API 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 일부 테이블 성능 향상 및 무결성 확보를 위한 테이블 비정규화 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 창고(INVENTORY) 기능 API 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 소비자 API - 회원/주소관리 API 통합/기능연동 및 테스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 농작물/상품관리 API 통합/기능연동 및 테스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 관리자API 상품 등록 로직 개선</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 페이지</t>
+  </si>
+  <si>
+    <t>/account/login</t>
+  </si>
+  <si>
+    <t>로그인 화면 반환</t>
+  </si>
+  <si>
+    <t>회원가입 페이지</t>
+  </si>
+  <si>
+    <t>/account/register</t>
+  </si>
+  <si>
+    <t>회원가입 화면 반환</t>
+  </si>
+  <si>
+    <t>ACTION</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>행동</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>/api/account/login</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>본문: x-www-form-urlencoded(loginId, userPw) / 응답: "success" 또는 "fail" / 성공 시 세션에 userId 저장</t>
+  </si>
+  <si>
+    <t>로그아웃</t>
+  </si>
+  <si>
+    <t>/api/account/logout</t>
+  </si>
+  <si>
+    <t>세션 무효화 / 응답: "logout success" 또는 204</t>
+  </si>
+  <si>
+    <t>/api/account/register</t>
+  </si>
+  <si>
+    <t>본문: x-www-form-urlencoded(...) / 응답: "success" 또는 "fail"</t>
+  </si>
+  <si>
+    <t>중복 아이디 체크</t>
+  </si>
+  <si>
+    <t>/api/account/idcheck</t>
+  </si>
+  <si>
+    <t>본문: x-www-form-urlencoded(loginId) / 응답: "dup" 또는 "unique"</t>
+  </si>
+  <si>
+    <t>/admin</t>
+  </si>
+  <si>
+    <t>/admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자API</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>계정API</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 전용 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>특정 농작물 조회</t>
+  </si>
+  <si>
+    <t>/{cropId}</t>
+  </si>
+  <si>
+    <t>전체 농작물 조회</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>농작물 추가</t>
+  </si>
+  <si>
+    <t>농작물 삭제</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>농작물 수정</t>
+  </si>
+  <si>
+    <t>농작물 활성화</t>
+  </si>
+  <si>
+    <t>/enable/{cropId}</t>
+  </si>
+  <si>
+    <t>농작물 비활성화</t>
+  </si>
+  <si>
+    <t>/disable/{cropId}</t>
+  </si>
+  <si>
+    <t>비고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>행동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>API</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/shop</t>
+  </si>
+  <si>
+    <t>/shop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>농장 주소 관리 메서드 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주소 조회</t>
+  </si>
+  <si>
+    <t>주소 수정</t>
+  </si>
+  <si>
+    <t>/update</t>
+  </si>
+  <si>
+    <t>/admin/api/address</t>
+  </si>
+  <si>
+    <t>상품 목록 조회 (관리자 전용)</t>
+  </si>
+  <si>
+    <t>상품 등록 html</t>
+  </si>
+  <si>
+    <t>/shop/additem</t>
+  </si>
+  <si>
+    <t>상품 등록</t>
+  </si>
+  <si>
+    <t>상품 수정</t>
+  </si>
+  <si>
+    <t>/shop/item/{id}</t>
   </si>
   <si>
     <t>PUT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/orders</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/order/{id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/order/status/{id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PATCH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/order/cancel/{id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/products/search</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ex) /admin/products</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ex) /common/products</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주소 관리 메서드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주소 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/address</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주소 수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/address/{id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기능</t>
-  </si>
-  <si>
-    <t>페이지 명칭 (URL 예시)</t>
-  </si>
-  <si>
-    <t>역할 및 내용</t>
-  </si>
-  <si>
-    <t>로그인</t>
-  </si>
-  <si>
-    <t>로그인 폼</t>
-  </si>
-  <si>
-    <t>회원가입</t>
-  </si>
-  <si>
-    <t>회원가입 폼</t>
-  </si>
-  <si>
-    <t>index.html</t>
-  </si>
-  <si>
-    <t>메인 페이지, 주요 상품 노출</t>
-  </si>
-  <si>
-    <t>기능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>역할 및 내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>common/login.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>common/join.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공통파트 - 회원/로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0. 메인파트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장바구니</t>
-  </si>
-  <si>
-    <t>메인화면</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장바구니 내역 조회, 수량 변경, 일부/전체 주문 기능</t>
-  </si>
-  <si>
-    <t>상품 목록</t>
-  </si>
-  <si>
-    <t>product/list.html</t>
-  </si>
-  <si>
-    <t>상품 상세</t>
-  </si>
-  <si>
-    <t>product/detail.html</t>
-  </si>
-  <si>
-    <t>모든 농작물 목록, 검색 및 필터 기능 포함</t>
-  </si>
-  <si>
-    <t>단일 농작물 상세 정보, 장바구니 담기, Sold Out 표시</t>
-  </si>
-  <si>
-    <t>주문/결제</t>
-  </si>
-  <si>
-    <t>주문 내역 조회</t>
-  </si>
-  <si>
-    <t>주문 상세</t>
-  </si>
-  <si>
-    <t>특정 주문의 상세 정보</t>
-  </si>
-  <si>
-    <t>배송지 관리</t>
-  </si>
-  <si>
-    <t>배송지 추가/수정/삭제 폼</t>
-  </si>
-  <si>
-    <t>주문 내역 전체 조회, 취소 가능 상태 확인</t>
-  </si>
-  <si>
-    <t>관리자 홈</t>
-  </si>
-  <si>
-    <t>admin/dashboard.html</t>
-  </si>
-  <si>
-    <t>관리자 대시보드 (주요 통계 요약)</t>
-  </si>
-  <si>
-    <t>농작물 등록/관리</t>
-  </si>
-  <si>
-    <t>admin/farm/manage.html</t>
-  </si>
-  <si>
-    <t>농작물 추가/삭제/활성화/비활성화 폼 및 목록</t>
-  </si>
-  <si>
-    <t>상품 등록/관리</t>
-  </si>
-  <si>
-    <t>admin/product/manage.html</t>
-  </si>
-  <si>
-    <t>판매 상품 등록 및 게시 중단 기능 목록</t>
-  </si>
-  <si>
-    <t>주문 조회/처리</t>
-  </si>
-  <si>
-    <t>admin/order/list.html</t>
-  </si>
-  <si>
-    <t>통계/정산</t>
-  </si>
-  <si>
-    <t>admin/stats/main.html</t>
-  </si>
-  <si>
-    <t>일자별/품목별 통계, 정산 내역 조회</t>
-  </si>
-  <si>
-    <t>소비자 주문 목록 조회, 주문 상태 변경, 송장 번호 입력</t>
-  </si>
-  <si>
-    <t>페이지 명칭</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 사용자 파트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 관리자 파트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>담당자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결제, 주소지 정보 입력 주문 확정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>prontend_admin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>branch계정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>prontend_common</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>prontend_user</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>* GitHub_NamingRule</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>강승태</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공통화면</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>base.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공통 헤더/푸터 파트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>허정우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장경국</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>product/cart.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>product/checkout.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>product/orderList.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>product/orderDetail.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>product/address.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사용자파트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자파트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마이페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메인페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>대</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>중</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품목록</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품상세</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장바구니</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품제거</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>구매</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>배송정보입력(옵션)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결제하기(주문결제)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>선택상품주문</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전체상품주문</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일반로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원가입</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>배송지수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>배송지추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>배송지삭제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주문배송관리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상세보기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주문취소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주문하기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원/로그인</t>
-  </si>
-  <si>
-    <t>회원가입 기능</t>
-  </si>
-  <si>
-    <t>로그인 기능</t>
-  </si>
-  <si>
-    <t>관리자 계정으로 로그인 하면 관리 사이트로 넘어간다.</t>
-  </si>
-  <si>
-    <t>상품/농작물 등록·관리</t>
-  </si>
-  <si>
-    <t>농작물 추가 기능</t>
-  </si>
-  <si>
-    <t>농작물 삭제 기능</t>
-  </si>
-  <si>
-    <t>농작물 재배 활성화/비활성화 기능</t>
-  </si>
-  <si>
-    <t>상품 등록 및 관리</t>
-  </si>
-  <si>
-    <t>창고에 있는 만큼의 농작물을 등록할 수 있다.</t>
-  </si>
-  <si>
-    <t>등록되어 있는 농작물은 게시를 중단할 수 있다.</t>
-  </si>
-  <si>
-    <t>검색/탐색</t>
-  </si>
-  <si>
-    <t>상품 검색 기능 (수확시기 등으로 필터 적용)</t>
-  </si>
-  <si>
-    <t>판매 사이트에 올라와 있는 농작물을 볼 수 있다.</t>
-  </si>
-  <si>
-    <t>장바구니/주문·결제</t>
-  </si>
-  <si>
-    <t>상품 장바구니 기능</t>
-  </si>
-  <si>
-    <t>농작물의 페이지로 들어가 개수를 지정해서 장바구니에 담을 수 있다.</t>
-  </si>
-  <si>
-    <t>장바구니에 있는 농작물의 일부 혹은 전부 구매할 수 있다.</t>
-  </si>
-  <si>
-    <t>주문 조회/처리 - (관리자)</t>
-  </si>
-  <si>
-    <t>소비자가 주문한 농작물 조회 기능</t>
-  </si>
-  <si>
-    <t>주문 상태 변경 기능 → 배송 중으로 변경</t>
-  </si>
-  <si>
-    <t>배송 처리(주문 상품별 송장 번호 및 택배사 정보 입력)</t>
-  </si>
-  <si>
-    <t>주문 조회/처리(취소) - (사용자)</t>
-  </si>
-  <si>
-    <t>재고/노출 관리 - (사용자)</t>
-  </si>
-  <si>
-    <t>통계/정산 - (관리자)</t>
-  </si>
-  <si>
-    <t>농작물 주문 통계 기능 (일자별/품목별 판매시 cnt++)</t>
-  </si>
-  <si>
-    <t>관리자</t>
-  </si>
-  <si>
-    <t>정산(판매 내역, 금액 조회)</t>
-  </si>
-  <si>
-    <t>계정/주소·계좌 관리</t>
-  </si>
-  <si>
-    <t>사용자</t>
-  </si>
-  <si>
-    <t>농가 정보, 계좌 등록</t>
-  </si>
-  <si>
-    <t>물품 상태가 배송 중으로 바뀌기 전에는 주문을 취소할 수 있다.</t>
-  </si>
-  <si>
-    <t>요구 사항 정리</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (품절 표기는 재고/노출과 연관, 배송 맥락과 함께 노출되는 문구로 함께 묶음)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일반 사용자는 판매 페이지에서 재고가 없는 농작물은 자동으로 sold out 처리된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>●</t>
-  </si>
-  <si>
-    <t>●</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>☞</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>항목</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>월</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기획</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주제선정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>디자인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기능구현</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>통합테스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4주차</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1주차</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>월</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>목</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>금</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>토</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Login/Register</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2주차</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3주차</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>월</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>목</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>설계</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>요구사항 및 UseCase 설계</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DB &amp; ERD Design</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>API 및 각 파트별 기능설계</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Display Design</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSS Design</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>API Controller</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Service</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Manager</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JavaScript/JQuery</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MyBatis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User purchase order/cart</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shop Item Searching</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Order Managing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Crops / Inventories managing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Statistics</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Troubleshooting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장바구니에서 아이템 구매</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장바구니에서 아이템 삭제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주문 결과 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/orderlist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품 구매 기능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사용자는 구매한 물품의 총 개수와 가격을 확인하여 구매할 수 있다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>소비자는 구매한 물품의 총 개수와 가격을 조회할 수 있다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>소비자가 주문한 주문 내역 조회/취소 기능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/cart</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주문 목록 조회</t>
-  </si>
-  <si>
-    <t>/orders</t>
-  </si>
-  <si>
-    <t>GET</t>
-  </si>
-  <si>
-    <t>장바구니에 아이템 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 삭제</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1350,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1507,13 +1691,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1730,6 +1925,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1751,17 +1955,32 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="31" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2094,7 +2313,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2102,10 +2321,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="14"/>
+  </cols>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O80"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2169,513 +2406,821 @@
       <c r="N3" s="66"/>
       <c r="O3" s="66"/>
     </row>
-    <row r="4" spans="1:15" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+    <row r="4" spans="1:15" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" ht="27" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="84" t="s">
+        <v>251</v>
+      </c>
       <c r="B6" s="5" t="s">
-        <v>3</v>
+        <v>252</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>8</v>
+        <v>229</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>32</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E8" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:15" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="84" t="s">
+        <v>254</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E13" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="A15" s="88" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="88" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="89"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="89"/>
+    </row>
+    <row r="16" spans="1:15" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="67"/>
+      <c r="M21" s="67"/>
+      <c r="N21" s="67"/>
+      <c r="O21" s="67"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="67"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="67"/>
+      <c r="M22" s="67"/>
+      <c r="N22" s="67"/>
+      <c r="O22" s="67"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="67"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="67"/>
+      <c r="M23" s="67"/>
+      <c r="N23" s="67"/>
+      <c r="O23" s="67"/>
+    </row>
+    <row r="24" spans="1:15" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:15" ht="21" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="85"/>
+      <c r="B25" s="85"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="86"/>
+    </row>
+    <row r="26" spans="1:15" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:15" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:15" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="67"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="67"/>
-      <c r="N15" s="67"/>
-      <c r="O15" s="67"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="67"/>
-      <c r="B16" s="67"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="67"/>
-      <c r="N16" s="67"/>
-      <c r="O16" s="67"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="67"/>
-      <c r="B17" s="67"/>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="67"/>
-      <c r="L17" s="67"/>
-      <c r="M17" s="67"/>
-      <c r="N17" s="67"/>
-      <c r="O17" s="67"/>
-    </row>
-    <row r="18" spans="1:15" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A27" s="85" t="s">
+        <v>276</v>
+      </c>
+      <c r="B27" s="90" t="s">
+        <v>272</v>
+      </c>
+      <c r="C27" s="86" t="s">
+        <v>229</v>
+      </c>
+      <c r="D27" s="86" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A28" s="85"/>
+      <c r="B28" s="85"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="86"/>
+    </row>
+    <row r="29" spans="1:15" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:15" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:15" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:15" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>278</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>20</v>
+        <v>279</v>
+      </c>
+      <c r="C31" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>280</v>
+      </c>
+      <c r="B32" t="s">
+        <v>281</v>
+      </c>
+      <c r="C32" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>282</v>
+      </c>
+      <c r="B33" t="s">
+        <v>281</v>
+      </c>
+      <c r="C33" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>283</v>
+      </c>
+      <c r="B34" t="s">
+        <v>279</v>
+      </c>
+      <c r="C34" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>285</v>
+      </c>
+      <c r="B35" t="s">
+        <v>279</v>
+      </c>
+      <c r="C35" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>286</v>
+      </c>
+      <c r="B36" t="s">
+        <v>287</v>
+      </c>
+      <c r="C36" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>288</v>
+      </c>
+      <c r="B37" t="s">
+        <v>289</v>
+      </c>
+      <c r="C37" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>258</v>
+      </c>
+      <c r="B42" t="s">
+        <v>259</v>
+      </c>
+      <c r="C42" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>298</v>
+      </c>
+      <c r="B43" t="s">
+        <v>281</v>
+      </c>
+      <c r="C43" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>299</v>
+      </c>
+      <c r="B44" t="s">
+        <v>300</v>
+      </c>
+      <c r="C44" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:4" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>302</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>303</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>305</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>306</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>309</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+    </row>
+    <row r="54" spans="1:15" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="1:15" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" t="s">
+        <v>29</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" t="s">
+        <v>31</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C59" s="4"/>
+    </row>
+    <row r="62" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62" s="68"/>
+      <c r="C62" s="68"/>
+      <c r="D62" s="68"/>
+      <c r="E62" s="68"/>
+      <c r="F62" s="68"/>
+      <c r="G62" s="68"/>
+      <c r="H62" s="68"/>
+      <c r="I62" s="68"/>
+      <c r="J62" s="68"/>
+      <c r="K62" s="68"/>
+      <c r="L62" s="68"/>
+      <c r="M62" s="68"/>
+      <c r="N62" s="68"/>
+      <c r="O62" s="68"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A63" s="68"/>
+      <c r="B63" s="68"/>
+      <c r="C63" s="68"/>
+      <c r="D63" s="68"/>
+      <c r="E63" s="68"/>
+      <c r="F63" s="68"/>
+      <c r="G63" s="68"/>
+      <c r="H63" s="68"/>
+      <c r="I63" s="68"/>
+      <c r="J63" s="68"/>
+      <c r="K63" s="68"/>
+      <c r="L63" s="68"/>
+      <c r="M63" s="68"/>
+      <c r="N63" s="68"/>
+      <c r="O63" s="68"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A64" s="68"/>
+      <c r="B64" s="68"/>
+      <c r="C64" s="68"/>
+      <c r="D64" s="68"/>
+      <c r="E64" s="68"/>
+      <c r="F64" s="68"/>
+      <c r="G64" s="68"/>
+      <c r="H64" s="68"/>
+      <c r="I64" s="68"/>
+      <c r="J64" s="68"/>
+      <c r="K64" s="68"/>
+      <c r="L64" s="68"/>
+      <c r="M64" s="68"/>
+      <c r="N64" s="68"/>
+      <c r="O64" s="68"/>
+    </row>
+    <row r="65" spans="1:4" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+    </row>
+    <row r="67" spans="1:4" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" t="s">
+        <v>21</v>
+      </c>
+      <c r="C67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>230</v>
+      </c>
+      <c r="B68" t="s">
+        <v>23</v>
+      </c>
+      <c r="C68" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>218</v>
+      </c>
+      <c r="B69" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>217</v>
+      </c>
+      <c r="B70" t="s">
+        <v>226</v>
+      </c>
+      <c r="C70" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" s="3"/>
+    </row>
+    <row r="73" spans="1:4" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>220</v>
+      </c>
+      <c r="B73" t="s">
+        <v>221</v>
+      </c>
+      <c r="C73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>227</v>
+      </c>
+      <c r="B74" t="s">
+        <v>228</v>
+      </c>
+      <c r="C74" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>25</v>
+      </c>
+      <c r="B75" t="s">
+        <v>30</v>
+      </c>
+      <c r="C75" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>26</v>
+      </c>
+      <c r="B76" t="s">
+        <v>33</v>
+      </c>
+      <c r="C76" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B78" s="2"/>
+      <c r="C78" s="3"/>
+    </row>
+    <row r="79" spans="1:4" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>37</v>
+      </c>
+      <c r="B79" t="s">
+        <v>38</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>39</v>
       </c>
-      <c r="B32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C34" s="4"/>
-    </row>
-    <row r="37" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="68" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37" s="68"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="68"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="68"/>
-      <c r="J37" s="68"/>
-      <c r="K37" s="68"/>
-      <c r="L37" s="68"/>
-      <c r="M37" s="68"/>
-      <c r="N37" s="68"/>
-      <c r="O37" s="68"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A38" s="68"/>
-      <c r="B38" s="68"/>
-      <c r="C38" s="68"/>
-      <c r="D38" s="68"/>
-      <c r="E38" s="68"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="68"/>
-      <c r="K38" s="68"/>
-      <c r="L38" s="68"/>
-      <c r="M38" s="68"/>
-      <c r="N38" s="68"/>
-      <c r="O38" s="68"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A39" s="68"/>
-      <c r="B39" s="68"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="68"/>
-      <c r="F39" s="68"/>
-      <c r="G39" s="68"/>
-      <c r="H39" s="68"/>
-      <c r="I39" s="68"/>
-      <c r="J39" s="68"/>
-      <c r="K39" s="68"/>
-      <c r="L39" s="68"/>
-      <c r="M39" s="68"/>
-      <c r="N39" s="68"/>
-      <c r="O39" s="68"/>
-    </row>
-    <row r="40" spans="1:15" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="3"/>
-    </row>
-    <row r="42" spans="1:15" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B42" t="s">
-        <v>35</v>
-      </c>
-      <c r="C42" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B43" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>239</v>
-      </c>
-      <c r="B44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>238</v>
-      </c>
-      <c r="B45" t="s">
-        <v>247</v>
-      </c>
-      <c r="C45" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="3"/>
-    </row>
-    <row r="48" spans="1:15" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>241</v>
-      </c>
-      <c r="B48" t="s">
-        <v>242</v>
-      </c>
-      <c r="C48" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>248</v>
-      </c>
-      <c r="B49" t="s">
-        <v>249</v>
-      </c>
-      <c r="C49" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>39</v>
-      </c>
-      <c r="B50" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="B80" t="s">
         <v>40</v>
       </c>
-      <c r="B51" t="s">
-        <v>53</v>
-      </c>
-      <c r="C51" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="3"/>
-    </row>
-    <row r="54" spans="1:3" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>58</v>
-      </c>
-      <c r="B54" t="s">
-        <v>59</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>60</v>
-      </c>
-      <c r="B55" t="s">
-        <v>61</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>8</v>
+      <c r="C80" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:O3"/>
-    <mergeCell ref="A15:O17"/>
-    <mergeCell ref="A37:O39"/>
+    <mergeCell ref="A21:O23"/>
+    <mergeCell ref="A62:O64"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N34" sqref="A12:O34"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2694,7 +3239,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="65" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
@@ -2747,91 +3292,91 @@
     </row>
     <row r="5" spans="1:19" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="D7" s="70" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="D8" s="70"/>
       <c r="G8" s="11" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="D9" s="70"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D10" s="70"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="65" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="B12" s="65"/>
       <c r="C12" s="65"/>
@@ -2884,163 +3429,163 @@
     </row>
     <row r="15" spans="1:19" ht="24" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="Q16" s="69" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="R16" s="69"/>
       <c r="S16" s="4" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="D17" s="70" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="Q17" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="S17" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="R17" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="S17" s="4" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="D18" s="70"/>
       <c r="S18" s="6" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="D19" s="70"/>
       <c r="Q19" s="6" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="S19" s="6" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="D20" s="70"/>
       <c r="S20" s="6" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="D21" s="70"/>
       <c r="S21" s="6" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="D22" s="70"/>
       <c r="S22" s="6" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="D23" s="70"/>
       <c r="Q23" s="6" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="S23" s="6" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="S24" s="6" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="65" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="B25" s="65"/>
       <c r="C25" s="65"/>
@@ -3057,10 +3602,10 @@
       <c r="N25" s="65"/>
       <c r="O25" s="65"/>
       <c r="Q25" s="6" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="S25" s="6" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
@@ -3080,7 +3625,7 @@
       <c r="N26" s="65"/>
       <c r="O26" s="65"/>
       <c r="S26" s="6" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
@@ -3100,111 +3645,111 @@
       <c r="N27" s="65"/>
       <c r="O27" s="65"/>
       <c r="Q27" s="6" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="S27" s="6" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="24" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q28" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="Q28" s="6" t="s">
+      <c r="S28" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="S28" s="6" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="S29" s="6" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="D30" s="70" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="S30" s="6" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="D31" s="70"/>
       <c r="R31" s="6" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="S31" s="6" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="D32" s="70"/>
       <c r="S32" s="6" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="D33" s="70"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="D34" s="70"/>
     </row>
@@ -3224,7 +3769,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:X29"/>
   <sheetViews>
@@ -3239,7 +3784,7 @@
   <sheetData>
     <row r="3" spans="2:24" ht="72" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="71" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="C3" s="71"/>
       <c r="D3" s="71"/>
@@ -3288,10 +3833,10 @@
     </row>
     <row r="5" spans="2:24" ht="24" x14ac:dyDescent="0.3">
       <c r="D5" s="25" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
@@ -3302,10 +3847,10 @@
       <c r="L5" s="20"/>
       <c r="M5" s="20"/>
       <c r="N5" s="26" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="O5" s="19" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="P5" s="20"/>
       <c r="Q5" s="20"/>
@@ -3319,10 +3864,10 @@
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
       <c r="D6" s="18"/>
       <c r="E6" s="26" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
@@ -3333,10 +3878,10 @@
       <c r="M6" s="20"/>
       <c r="N6" s="20"/>
       <c r="O6" s="26" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="P6" s="27" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="Q6" s="20"/>
       <c r="R6" s="20"/>
@@ -3349,10 +3894,10 @@
     <row r="7" spans="2:24" x14ac:dyDescent="0.3">
       <c r="D7" s="18"/>
       <c r="E7" s="26" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
@@ -3364,7 +3909,7 @@
       <c r="N7" s="20"/>
       <c r="O7" s="20"/>
       <c r="P7" s="20" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="Q7" s="20"/>
       <c r="R7" s="20"/>
@@ -3378,7 +3923,7 @@
       <c r="D8" s="18"/>
       <c r="E8" s="26"/>
       <c r="F8" s="20" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
@@ -3390,7 +3935,7 @@
       <c r="N8" s="20"/>
       <c r="O8" s="20"/>
       <c r="P8" s="20" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="Q8" s="20"/>
       <c r="R8" s="20"/>
@@ -3424,10 +3969,10 @@
     </row>
     <row r="10" spans="2:24" ht="24" x14ac:dyDescent="0.3">
       <c r="D10" s="25" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
@@ -3438,10 +3983,10 @@
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="26" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="P10" s="20"/>
       <c r="Q10" s="20"/>
@@ -3455,10 +4000,10 @@
     <row r="11" spans="2:24" x14ac:dyDescent="0.3">
       <c r="D11" s="18"/>
       <c r="E11" s="26" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
@@ -3469,10 +4014,10 @@
       <c r="M11" s="20"/>
       <c r="N11" s="20"/>
       <c r="O11" s="26" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="P11" s="27" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="Q11" s="20"/>
       <c r="R11" s="20"/>
@@ -3485,10 +4030,10 @@
     <row r="12" spans="2:24" x14ac:dyDescent="0.3">
       <c r="D12" s="18"/>
       <c r="E12" s="26" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
@@ -3500,7 +4045,7 @@
       <c r="N12" s="20"/>
       <c r="O12" s="20"/>
       <c r="P12" s="14" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="Q12" s="20"/>
       <c r="R12" s="20"/>
@@ -3513,10 +4058,10 @@
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="D13" s="18"/>
       <c r="E13" s="26" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
@@ -3528,7 +4073,7 @@
       <c r="N13" s="20"/>
       <c r="O13" s="26"/>
       <c r="P13" s="20" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="Q13" s="20"/>
       <c r="R13" s="20"/>
@@ -3541,10 +4086,10 @@
     <row r="14" spans="2:24" x14ac:dyDescent="0.3">
       <c r="D14" s="18"/>
       <c r="E14" s="26" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
@@ -3565,7 +4110,7 @@
       <c r="D15" s="18"/>
       <c r="E15" s="20"/>
       <c r="F15" s="20" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
@@ -3575,10 +4120,10 @@
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
       <c r="N15" s="26" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="O15" s="19" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="P15" s="20"/>
       <c r="Q15" s="20"/>
@@ -3593,7 +4138,7 @@
       <c r="D16" s="18"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
@@ -3604,10 +4149,10 @@
       <c r="M16" s="20"/>
       <c r="N16" s="20"/>
       <c r="O16" s="26" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="P16" s="27" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="Q16" s="20"/>
       <c r="R16" s="20"/>
@@ -3631,7 +4176,7 @@
       <c r="N17" s="20"/>
       <c r="O17" s="20"/>
       <c r="P17" s="20" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="Q17" s="20"/>
       <c r="R17" s="20"/>
@@ -3643,10 +4188,10 @@
     </row>
     <row r="18" spans="4:23" ht="24" x14ac:dyDescent="0.3">
       <c r="D18" s="25" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
@@ -3670,10 +4215,10 @@
     <row r="19" spans="4:23" ht="24" x14ac:dyDescent="0.3">
       <c r="D19" s="18"/>
       <c r="E19" s="26" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
@@ -3683,10 +4228,10 @@
       <c r="L19" s="20"/>
       <c r="M19" s="20"/>
       <c r="N19" s="26" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="O19" s="19" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="P19" s="20"/>
       <c r="Q19" s="20"/>
@@ -3701,7 +4246,7 @@
       <c r="D20" s="18"/>
       <c r="E20" s="20"/>
       <c r="F20" s="27" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
@@ -3712,10 +4257,10 @@
       <c r="M20" s="20"/>
       <c r="N20" s="20"/>
       <c r="O20" s="26" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="P20" s="27" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="Q20" s="20"/>
       <c r="R20" s="20"/>
@@ -3739,7 +4284,7 @@
       <c r="N21" s="20"/>
       <c r="O21" s="20"/>
       <c r="P21" s="20" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="Q21" s="20"/>
       <c r="R21" s="20"/>
@@ -3751,10 +4296,10 @@
     </row>
     <row r="22" spans="4:23" ht="24" x14ac:dyDescent="0.3">
       <c r="D22" s="25" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
@@ -3766,10 +4311,10 @@
       <c r="M22" s="20"/>
       <c r="N22" s="20"/>
       <c r="O22" s="26" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="P22" s="27" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="Q22" s="20"/>
       <c r="R22" s="20"/>
@@ -3782,10 +4327,10 @@
     <row r="23" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D23" s="18"/>
       <c r="E23" s="26" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
@@ -3809,7 +4354,7 @@
       <c r="D24" s="18"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
@@ -3819,10 +4364,10 @@
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
       <c r="N24" s="26" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="O24" s="19" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="P24" s="20"/>
       <c r="Q24" s="20"/>
@@ -3837,7 +4382,7 @@
       <c r="D25" s="18"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
@@ -3849,7 +4394,7 @@
       <c r="N25" s="20"/>
       <c r="O25" s="20"/>
       <c r="P25" s="20" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="Q25" s="20"/>
       <c r="R25" s="20"/>
@@ -3862,10 +4407,10 @@
     <row r="26" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D26" s="18"/>
       <c r="E26" s="26" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="F26" s="27" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
@@ -3876,10 +4421,10 @@
       <c r="M26" s="20"/>
       <c r="N26" s="20"/>
       <c r="O26" s="26" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="P26" s="27" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="Q26" s="20"/>
       <c r="R26" s="20"/>
@@ -3892,7 +4437,7 @@
     <row r="27" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D27" s="18"/>
       <c r="F27" s="14" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
@@ -3904,7 +4449,7 @@
       <c r="N27" s="20"/>
       <c r="O27" s="20"/>
       <c r="P27" s="20" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="Q27" s="20"/>
       <c r="R27" s="20"/>
@@ -3925,10 +4470,10 @@
       <c r="M28" s="20"/>
       <c r="N28" s="20"/>
       <c r="O28" s="26" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="P28" s="27" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="Q28" s="20"/>
       <c r="R28" s="20"/>
@@ -3970,7 +4515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AE23"/>
   <sheetViews>
@@ -3978,7 +4523,7 @@
       <pane xSplit="30" ySplit="23" topLeftCell="AE24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AE1" sqref="AE1"/>
       <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3994,143 +4539,143 @@
     <row r="1" spans="2:31" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:31" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="72" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="75" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="75" t="s">
+        <v>185</v>
+      </c>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="75" t="s">
+        <v>195</v>
+      </c>
+      <c r="S3" s="76"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="76"/>
+      <c r="X3" s="77"/>
+      <c r="Y3" s="79" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z3" s="80"/>
+      <c r="AA3" s="80"/>
+      <c r="AB3" s="80"/>
+      <c r="AC3" s="80"/>
+      <c r="AD3" s="80"/>
+      <c r="AE3" s="81"/>
+    </row>
+    <row r="4" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="73"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" s="63" t="s">
+        <v>187</v>
+      </c>
+      <c r="F4" s="63" t="s">
+        <v>188</v>
+      </c>
+      <c r="G4" s="63" t="s">
+        <v>189</v>
+      </c>
+      <c r="H4" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="I4" s="63" t="s">
+        <v>191</v>
+      </c>
+      <c r="J4" s="63" t="s">
+        <v>196</v>
+      </c>
+      <c r="K4" s="63" t="s">
         <v>197</v>
       </c>
-      <c r="C3" s="72" t="s">
+      <c r="L4" s="63" t="s">
         <v>198</v>
       </c>
-      <c r="D3" s="72" t="s">
-        <v>206</v>
-      </c>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="75" t="s">
-        <v>215</v>
-      </c>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="Q3" s="74"/>
-      <c r="R3" s="72" t="s">
-        <v>216</v>
-      </c>
-      <c r="S3" s="73"/>
-      <c r="T3" s="73"/>
-      <c r="U3" s="73"/>
-      <c r="V3" s="73"/>
-      <c r="W3" s="73"/>
-      <c r="X3" s="74"/>
-      <c r="Y3" s="76" t="s">
-        <v>205</v>
-      </c>
-      <c r="Z3" s="77"/>
-      <c r="AA3" s="77"/>
-      <c r="AB3" s="77"/>
-      <c r="AC3" s="77"/>
-      <c r="AD3" s="77"/>
-      <c r="AE3" s="78"/>
-    </row>
-    <row r="4" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="80"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="63" t="s">
-        <v>207</v>
-      </c>
-      <c r="E4" s="63" t="s">
-        <v>208</v>
-      </c>
-      <c r="F4" s="63" t="s">
-        <v>209</v>
-      </c>
-      <c r="G4" s="63" t="s">
-        <v>210</v>
-      </c>
-      <c r="H4" s="63" t="s">
-        <v>211</v>
-      </c>
-      <c r="I4" s="63" t="s">
-        <v>212</v>
-      </c>
-      <c r="J4" s="63" t="s">
-        <v>217</v>
-      </c>
-      <c r="K4" s="63" t="s">
-        <v>218</v>
-      </c>
-      <c r="L4" s="63" t="s">
-        <v>219</v>
-      </c>
       <c r="M4" s="63" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="N4" s="63" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="O4" s="63" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="P4" s="63" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="Q4" s="63" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="R4" s="63" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="S4" s="63" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="T4" s="63" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="U4" s="63" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="V4" s="63" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="W4" s="63" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="X4" s="63" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="Y4" s="63" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="Z4" s="63" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="AA4" s="63" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="AB4" s="63" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="AC4" s="63" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="AD4" s="63" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="AE4" s="63" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="79" t="s">
-        <v>200</v>
+      <c r="B5" s="72" t="s">
+        <v>179</v>
       </c>
       <c r="C5" s="64" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="D5" s="42"/>
       <c r="E5" s="43"/>
@@ -4162,9 +4707,9 @@
       <c r="AE5" s="45"/>
     </row>
     <row r="6" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="80"/>
+      <c r="B6" s="73"/>
       <c r="C6" s="64" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="33"/>
@@ -4196,11 +4741,11 @@
       <c r="AE6" s="34"/>
     </row>
     <row r="7" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="79" t="s">
-        <v>221</v>
+      <c r="B7" s="72" t="s">
+        <v>200</v>
       </c>
       <c r="C7" s="64" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="D7" s="42"/>
       <c r="E7" s="43"/>
@@ -4232,9 +4777,9 @@
       <c r="AE7" s="45"/>
     </row>
     <row r="8" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="80"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="64" t="s">
-        <v>224</v>
+        <v>203</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="33"/>
@@ -4266,11 +4811,11 @@
       <c r="AE8" s="34"/>
     </row>
     <row r="9" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="79" t="s">
-        <v>202</v>
+      <c r="B9" s="72" t="s">
+        <v>181</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="D9" s="42"/>
       <c r="E9" s="43"/>
@@ -4302,9 +4847,9 @@
       <c r="AE9" s="45"/>
     </row>
     <row r="10" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="80"/>
+      <c r="B10" s="73"/>
       <c r="C10" s="64" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="33"/>
@@ -4336,11 +4881,11 @@
       <c r="AE10" s="34"/>
     </row>
     <row r="11" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="79" t="s">
-        <v>203</v>
+      <c r="B11" s="72" t="s">
+        <v>182</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="D11" s="42"/>
       <c r="E11" s="43"/>
@@ -4372,9 +4917,9 @@
       <c r="AE11" s="45"/>
     </row>
     <row r="12" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="82"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="64" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="D12" s="30"/>
       <c r="E12" s="28"/>
@@ -4406,9 +4951,9 @@
       <c r="AE12" s="31"/>
     </row>
     <row r="13" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="82"/>
+      <c r="B13" s="74"/>
       <c r="C13" s="64" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
       <c r="D13" s="30"/>
       <c r="E13" s="28"/>
@@ -4440,9 +4985,9 @@
       <c r="AE13" s="31"/>
     </row>
     <row r="14" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="82"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="64" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
       <c r="D14" s="30"/>
       <c r="E14" s="28"/>
@@ -4474,9 +5019,9 @@
       <c r="AE14" s="31"/>
     </row>
     <row r="15" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="80"/>
+      <c r="B15" s="73"/>
       <c r="C15" s="64" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
       <c r="D15" s="32"/>
       <c r="E15" s="33"/>
@@ -4508,11 +5053,11 @@
       <c r="AE15" s="34"/>
     </row>
     <row r="16" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="79" t="s">
-        <v>204</v>
+      <c r="B16" s="72" t="s">
+        <v>183</v>
       </c>
       <c r="C16" s="64" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="D16" s="42"/>
       <c r="E16" s="43"/>
@@ -4544,9 +5089,9 @@
       <c r="AE16" s="45"/>
     </row>
     <row r="17" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="82"/>
+      <c r="B17" s="74"/>
       <c r="C17" s="64" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
       <c r="D17" s="30"/>
       <c r="E17" s="28"/>
@@ -4578,9 +5123,9 @@
       <c r="AE17" s="31"/>
     </row>
     <row r="18" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="82"/>
+      <c r="B18" s="74"/>
       <c r="C18" s="64" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="D18" s="30"/>
       <c r="E18" s="28"/>
@@ -4612,9 +5157,9 @@
       <c r="AE18" s="31"/>
     </row>
     <row r="19" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="82"/>
+      <c r="B19" s="74"/>
       <c r="C19" s="64" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="D19" s="30"/>
       <c r="E19" s="28"/>
@@ -4646,9 +5191,9 @@
       <c r="AE19" s="31"/>
     </row>
     <row r="20" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="82"/>
+      <c r="B20" s="74"/>
       <c r="C20" s="64" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
       <c r="D20" s="30"/>
       <c r="E20" s="28"/>
@@ -4680,9 +5225,9 @@
       <c r="AE20" s="31"/>
     </row>
     <row r="21" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="82"/>
+      <c r="B21" s="74"/>
       <c r="C21" s="64" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
       <c r="D21" s="30"/>
       <c r="E21" s="28"/>
@@ -4714,9 +5259,9 @@
       <c r="AE21" s="31"/>
     </row>
     <row r="22" spans="2:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="80"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="64" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
       <c r="D22" s="32"/>
       <c r="E22" s="33"/>
@@ -4750,20 +5295,242 @@
     <row r="23" spans="2:31" ht="11.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="B16:B22"/>
     <mergeCell ref="D3:J3"/>
     <mergeCell ref="K3:Q3"/>
     <mergeCell ref="R3:X3"/>
     <mergeCell ref="Y3:AE3"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="B16:B22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="38" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="1.875" style="14" customWidth="1"/>
+    <col min="2" max="2" width="9" style="14"/>
+    <col min="3" max="3" width="17.125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+      <c r="C3" s="83">
+        <v>45971</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="14">
+        <v>2</v>
+      </c>
+      <c r="C4" s="83">
+        <v>45972</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="14">
+        <v>3</v>
+      </c>
+      <c r="C5" s="83">
+        <v>45972</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="14">
+        <v>4</v>
+      </c>
+      <c r="C6" s="83">
+        <v>45973</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="14">
+        <v>5</v>
+      </c>
+      <c r="C7" s="83">
+        <v>45973</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="14">
+        <v>6</v>
+      </c>
+      <c r="C8" s="83">
+        <v>45973</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="14">
+        <v>7</v>
+      </c>
+      <c r="C9" s="83">
+        <v>45973</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="14">
+        <v>8</v>
+      </c>
+      <c r="C10" s="83">
+        <v>45973</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="14">
+        <v>9</v>
+      </c>
+      <c r="C11" s="83">
+        <v>45974</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="14">
+        <v>10</v>
+      </c>
+      <c r="C12" s="83">
+        <v>45975</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="14">
+        <v>11</v>
+      </c>
+      <c r="C13" s="83">
+        <v>45975</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="14">
+        <v>12</v>
+      </c>
+      <c r="C14" s="83">
+        <v>45975</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="14">
+        <v>13</v>
+      </c>
+      <c r="C15" s="83">
+        <v>45978</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="14">
+        <v>14</v>
+      </c>
+      <c r="C16" s="83">
+        <v>45978</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="14">
+        <v>15</v>
+      </c>
+      <c r="C17" s="83">
+        <v>45978</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="14">
+        <v>16</v>
+      </c>
+      <c r="C18" s="83">
+        <v>45979</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="14">
+        <v>17</v>
+      </c>
+      <c r="C19" s="83">
+        <v>45979</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>248</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>